<commit_message>
Added updated aviation companies list
</commit_message>
<xml_diff>
--- a/AviationCompanies.xlsx
+++ b/AviationCompanies.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{82118FF6-28E4-4DD0-B712-82EF01776D76}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DD279C51-F0AC-4584-8CFE-AD48CDA24A61}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="198">
   <si>
     <t>Aer Lingus</t>
   </si>
@@ -247,15 +247,9 @@
     <t>FPG Amentum</t>
   </si>
   <si>
-    <t>FTE Jerez</t>
-  </si>
-  <si>
     <t>fpg-amentum.aero</t>
   </si>
   <si>
-    <t>ftejerez.com</t>
-  </si>
-  <si>
     <t>Genesis Aircraft Services</t>
   </si>
   <si>
@@ -278,6 +272,348 @@
   </si>
   <si>
     <t>htaerotech.com</t>
+  </si>
+  <si>
+    <t>IT Carlow</t>
+  </si>
+  <si>
+    <t>Irish Air Corps</t>
+  </si>
+  <si>
+    <t>Irish Aviation Authority</t>
+  </si>
+  <si>
+    <t>ISTAT</t>
+  </si>
+  <si>
+    <t>Cityjet</t>
+  </si>
+  <si>
+    <t>cityjet.com</t>
+  </si>
+  <si>
+    <t>itcarlow.ie</t>
+  </si>
+  <si>
+    <t>iaa.ie</t>
+  </si>
+  <si>
+    <t>istat.org</t>
+  </si>
+  <si>
+    <t>IASC Shannon</t>
+  </si>
+  <si>
+    <t>iasc.aero</t>
+  </si>
+  <si>
+    <t>ICBC Leasing</t>
+  </si>
+  <si>
+    <t>icbcleasing.com</t>
+  </si>
+  <si>
+    <t>Jackson Square Aviation</t>
+  </si>
+  <si>
+    <t>jsa.com</t>
+  </si>
+  <si>
+    <t>cdbaviation.aero</t>
+  </si>
+  <si>
+    <t>CDB Aviation</t>
+  </si>
+  <si>
+    <t>Karman Aviation</t>
+  </si>
+  <si>
+    <t>karmanaviation.ie</t>
+  </si>
+  <si>
+    <t>KPMG</t>
+  </si>
+  <si>
+    <t>kpmg.ie</t>
+  </si>
+  <si>
+    <t>CloudCards</t>
+  </si>
+  <si>
+    <t>cloudcards.ie</t>
+  </si>
+  <si>
+    <t>Eirtech Aviation Services</t>
+  </si>
+  <si>
+    <t>eirtechaviation.ie</t>
+  </si>
+  <si>
+    <t>Irish Aviation Students Association</t>
+  </si>
+  <si>
+    <t>iasa.aero</t>
+  </si>
+  <si>
+    <t>Orix Aviation</t>
+  </si>
+  <si>
+    <t>orixaviation.com</t>
+  </si>
+  <si>
+    <t>PwC</t>
+  </si>
+  <si>
+    <t>pwc.ie</t>
+  </si>
+  <si>
+    <t>Ryanair</t>
+  </si>
+  <si>
+    <t>ryanair.com</t>
+  </si>
+  <si>
+    <t>Swissport</t>
+  </si>
+  <si>
+    <t>Menzies Aviation</t>
+  </si>
+  <si>
+    <t>menziesaviation.com</t>
+  </si>
+  <si>
+    <t>swissport.com</t>
+  </si>
+  <si>
+    <t>Sky Handling Partner</t>
+  </si>
+  <si>
+    <t>skyhandlingpartner.ie</t>
+  </si>
+  <si>
+    <t>Law Society of Ireland</t>
+  </si>
+  <si>
+    <t>lawsociety.ie</t>
+  </si>
+  <si>
+    <t>LCETB</t>
+  </si>
+  <si>
+    <t>limerickclare.etb.ie</t>
+  </si>
+  <si>
+    <t>National Flight Centre</t>
+  </si>
+  <si>
+    <t>nfc.ie</t>
+  </si>
+  <si>
+    <t>Nordic Aviation Capital</t>
+  </si>
+  <si>
+    <t>nac.dk</t>
+  </si>
+  <si>
+    <t>Part M Aviation</t>
+  </si>
+  <si>
+    <t>partmaviation.com</t>
+  </si>
+  <si>
+    <t>Grant Thornton</t>
+  </si>
+  <si>
+    <t>SMBC Aviation Capital</t>
+  </si>
+  <si>
+    <t>smbc.aero</t>
+  </si>
+  <si>
+    <t>DMS Governance</t>
+  </si>
+  <si>
+    <t>irelandiaaviation.ie</t>
+  </si>
+  <si>
+    <t>Irelandia Aviation</t>
+  </si>
+  <si>
+    <t>grantthornton.ie</t>
+  </si>
+  <si>
+    <t>dmsgovernance.com</t>
+  </si>
+  <si>
+    <t>Matheson</t>
+  </si>
+  <si>
+    <t>matheson.com</t>
+  </si>
+  <si>
+    <t>Shannon IASC</t>
+  </si>
+  <si>
+    <t>Shannon Airport</t>
+  </si>
+  <si>
+    <t>shannonairport.ie</t>
+  </si>
+  <si>
+    <t>CALC</t>
+  </si>
+  <si>
+    <t>calc.com.hk</t>
+  </si>
+  <si>
+    <t>Macquarie</t>
+  </si>
+  <si>
+    <t>macquarie.com</t>
+  </si>
+  <si>
+    <t>MC Aviation Partners</t>
+  </si>
+  <si>
+    <t>mcapgroup.com</t>
+  </si>
+  <si>
+    <t>Merx Aviation</t>
+  </si>
+  <si>
+    <t>merxaviation.com</t>
+  </si>
+  <si>
+    <t>Skyworks Capital</t>
+  </si>
+  <si>
+    <t>skyworkscapital.com</t>
+  </si>
+  <si>
+    <t>BOC Aviation</t>
+  </si>
+  <si>
+    <t>bocaviation.com</t>
+  </si>
+  <si>
+    <t>Maples</t>
+  </si>
+  <si>
+    <t>maplesandcalder.com</t>
+  </si>
+  <si>
+    <t>Stellwagen Group</t>
+  </si>
+  <si>
+    <t>stellwagengroup.com</t>
+  </si>
+  <si>
+    <t>Mason Hayes  Curran</t>
+  </si>
+  <si>
+    <t>mhc.ie</t>
+  </si>
+  <si>
+    <t>Sysco Leasing Software</t>
+  </si>
+  <si>
+    <t>leasing.sysco-software.com</t>
+  </si>
+  <si>
+    <t>Flying in Ireland</t>
+  </si>
+  <si>
+    <t>flyinginireland.com</t>
+  </si>
+  <si>
+    <t>Norwegian Air International</t>
+  </si>
+  <si>
+    <t>norwegian.com</t>
+  </si>
+  <si>
+    <t>CHC Helicopters</t>
+  </si>
+  <si>
+    <t>chcheli.com</t>
+  </si>
+  <si>
+    <t>Newcastle Airfield</t>
+  </si>
+  <si>
+    <t>einc.ie</t>
+  </si>
+  <si>
+    <t>Weston Airport</t>
+  </si>
+  <si>
+    <t>westonairport.ie</t>
+  </si>
+  <si>
+    <t>Ireland West Airport</t>
+  </si>
+  <si>
+    <t>irelandwestairport.com</t>
+  </si>
+  <si>
+    <t>Sligo Airport</t>
+  </si>
+  <si>
+    <t>sligoairport.com</t>
+  </si>
+  <si>
+    <t>Donegal Airport</t>
+  </si>
+  <si>
+    <t>donegalairport.ie</t>
+  </si>
+  <si>
+    <t>Sita</t>
+  </si>
+  <si>
+    <t>sita.aero</t>
+  </si>
+  <si>
+    <t>Lufthansa Technik</t>
+  </si>
+  <si>
+    <t>lufthansa-technik.com</t>
+  </si>
+  <si>
+    <t>Trim Flying Club</t>
+  </si>
+  <si>
+    <t>trimflyingclub.ie</t>
+  </si>
+  <si>
+    <t>skydive.ie</t>
+  </si>
+  <si>
+    <t>Irish Parachute Club</t>
+  </si>
+  <si>
+    <t>Kerry Airport</t>
+  </si>
+  <si>
+    <t>kerryairport.ie</t>
+  </si>
+  <si>
+    <t>Waterford Airport</t>
+  </si>
+  <si>
+    <t>waterfordairport.ie</t>
+  </si>
+  <si>
+    <t>University of Limerick</t>
+  </si>
+  <si>
+    <t>ul.ie</t>
+  </si>
+  <si>
+    <t>UCD</t>
+  </si>
+  <si>
+    <t>ucd.ie</t>
   </si>
 </sst>
 </file>
@@ -595,15 +931,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -793,162 +1129,615 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>156</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>146</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>170</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B33" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>66</v>
+        <v>180</v>
       </c>
       <c r="B37" t="s">
-        <v>70</v>
+        <v>181</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>136</v>
       </c>
       <c r="B38" t="s">
-        <v>76</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B41" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>66</v>
+      </c>
+      <c r="B46" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>166</v>
+      </c>
+      <c r="B47" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>78</v>
+      </c>
+      <c r="B49" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>76</v>
+      </c>
+      <c r="B50" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B52" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>82</v>
+      </c>
+      <c r="B53" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>93</v>
+      </c>
+      <c r="B54" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>95</v>
+      </c>
+      <c r="B55" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>176</v>
+      </c>
+      <c r="B56" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>86</v>
+      </c>
+      <c r="B58" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>109</v>
+      </c>
+      <c r="B59" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>189</v>
+      </c>
+      <c r="B60" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>138</v>
+      </c>
+      <c r="B61" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>87</v>
+      </c>
+      <c r="B62" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>84</v>
       </c>
-      <c r="B43" t="s">
-        <v>85</v>
+      <c r="B63" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>97</v>
+      </c>
+      <c r="B64" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>101</v>
+      </c>
+      <c r="B65" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>190</v>
+      </c>
+      <c r="B66" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>103</v>
+      </c>
+      <c r="B67" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>123</v>
+      </c>
+      <c r="B68" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>125</v>
+      </c>
+      <c r="B69" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>184</v>
+      </c>
+      <c r="B70" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>148</v>
+      </c>
+      <c r="B71" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>158</v>
+      </c>
+      <c r="B72" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>162</v>
+      </c>
+      <c r="B73" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>141</v>
+      </c>
+      <c r="B74" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>150</v>
+      </c>
+      <c r="B75" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>118</v>
+      </c>
+      <c r="B76" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>172</v>
+      </c>
+      <c r="B78" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>127</v>
+      </c>
+      <c r="B79" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>129</v>
+      </c>
+      <c r="B80" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>168</v>
+      </c>
+      <c r="B81" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>111</v>
+      </c>
+      <c r="B82" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>131</v>
+      </c>
+      <c r="B83" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>113</v>
+      </c>
+      <c r="B84" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>115</v>
+      </c>
+      <c r="B85" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>144</v>
+      </c>
+      <c r="B86" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>143</v>
+      </c>
+      <c r="B87" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>182</v>
+      </c>
+      <c r="B88" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>121</v>
+      </c>
+      <c r="B89" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>154</v>
+      </c>
+      <c r="B90" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>178</v>
+      </c>
+      <c r="B91" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>134</v>
+      </c>
+      <c r="B92" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>160</v>
+      </c>
+      <c r="B93" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>117</v>
+      </c>
+      <c r="B94" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>164</v>
+      </c>
+      <c r="B95" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>186</v>
+      </c>
+      <c r="B96" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>196</v>
+      </c>
+      <c r="B97" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>194</v>
+      </c>
+      <c r="B98" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>174</v>
+      </c>
+      <c r="B99" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>192</v>
+      </c>
+      <c r="B100" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>